<commit_message>
PBAC methods and locators WIP
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/PBACPermissions.xlsx
+++ b/InputFiles/CRDC/PBACPermissions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/CRDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17332937-907D-944B-BD0E-58D795B7680F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC5ED49-1292-D040-AC5E-5867754BE5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="3680" windowWidth="27240" windowHeight="16440" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
+    <workbookView xWindow="3020" yWindow="-26520" windowWidth="27240" windowHeight="16440" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
   </bookViews>
   <sheets>
     <sheet name="Permissions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="115">
   <si>
     <t>Group</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Federal Lead</t>
-  </si>
-  <si>
-    <t>Data Commons Personnel</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -219,6 +213,174 @@
   </si>
   <si>
     <t>access:request</t>
+  </si>
+  <si>
+    <t>Fedlead</t>
+  </si>
+  <si>
+    <t>Dcp</t>
+  </si>
+  <si>
+    <t>When available for review</t>
+  </si>
+  <si>
+    <t>Submission Request is ready for review</t>
+  </si>
+  <si>
+    <t>submission_request:to_be_reviewed</t>
+  </si>
+  <si>
+    <t>When review decision made</t>
+  </si>
+  <si>
+    <t>Submission Request review decision</t>
+  </si>
+  <si>
+    <t>submission_request:reviewed</t>
+  </si>
+  <si>
+    <t>When canceled/restored</t>
+  </si>
+  <si>
+    <t>Submission Request Canceled or Restored</t>
+  </si>
+  <si>
+    <t>submission_request:canceled</t>
+  </si>
+  <si>
+    <t>When expiring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submission Request is expiring </t>
+  </si>
+  <si>
+    <t>submission_request:expiring</t>
+  </si>
+  <si>
+    <t>When deleted</t>
+  </si>
+  <si>
+    <t>Submission Request Deleted</t>
+  </si>
+  <si>
+    <t>submission_request:deleted</t>
+  </si>
+  <si>
+    <t>When created</t>
+  </si>
+  <si>
+    <t>Data Submission is created</t>
+  </si>
+  <si>
+    <t>data_submission:created</t>
+  </si>
+  <si>
+    <t>Data Submission Emails</t>
+  </si>
+  <si>
+    <t>When submitted</t>
+  </si>
+  <si>
+    <t>Data Submission is submitted</t>
+  </si>
+  <si>
+    <t>data_submission:submitted</t>
+  </si>
+  <si>
+    <t>When cancelled</t>
+  </si>
+  <si>
+    <t>Data Submission is cancelled</t>
+  </si>
+  <si>
+    <t>data_submission:cancelled</t>
+  </si>
+  <si>
+    <t>When withdrawn</t>
+  </si>
+  <si>
+    <t>Data Submission is withdrawn</t>
+  </si>
+  <si>
+    <t>data_submission:withdrawn</t>
+  </si>
+  <si>
+    <t>When released</t>
+  </si>
+  <si>
+    <t>Data Submission is released</t>
+  </si>
+  <si>
+    <t>data_submission:released</t>
+  </si>
+  <si>
+    <t>When rejected</t>
+  </si>
+  <si>
+    <t>Data Submission is rejected</t>
+  </si>
+  <si>
+    <t>data_submission:rejected</t>
+  </si>
+  <si>
+    <t>When completed</t>
+  </si>
+  <si>
+    <t>Data Submission is completed</t>
+  </si>
+  <si>
+    <t>data_submission:completed</t>
+  </si>
+  <si>
+    <t>Data Submission is expiing</t>
+  </si>
+  <si>
+    <t>data_submission:expiring</t>
+  </si>
+  <si>
+    <t>Data Submission is deleted</t>
+  </si>
+  <si>
+    <t>data_submission:deleted</t>
+  </si>
+  <si>
+    <t>access:requested</t>
+  </si>
+  <si>
+    <t>Account Access Change</t>
+  </si>
+  <si>
+    <t>account:access_changed</t>
+  </si>
+  <si>
+    <t>Account Disabled</t>
+  </si>
+  <si>
+    <t>Account Disabled  (by system and by admin)</t>
+  </si>
+  <si>
+    <t>account:inactivated</t>
+  </si>
+  <si>
+    <t>Account Disabled (Consolidated)</t>
+  </si>
+  <si>
+    <t>Account Disabled  (consolidated)</t>
+  </si>
+  <si>
+    <t>account:users_inactivated</t>
+  </si>
+  <si>
+    <t>Submission Request Emails</t>
+  </si>
+  <si>
+    <t>When Submitted</t>
+  </si>
+  <si>
+    <t>Submission Request is received</t>
+  </si>
+  <si>
+    <t>submission_request:submitted</t>
   </si>
 </sst>
 </file>
@@ -590,13 +752,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77EC54C-AF12-1945-AE96-F02A9C2EB52A}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -609,515 +778,1066 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
         <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
         <v>55</v>
-      </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" t="s">
         <v>58</v>
       </c>
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" t="s">
-        <v>60</v>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add self PBAC defaults verification
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/PBACPermissions.xlsx
+++ b/InputFiles/CRDC/PBACPermissions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/CRDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D214CE-302B-3C49-A990-8744B9B95975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2854D568-76A7-6045-ABF4-E58D84C305F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17440" yWindow="-26000" windowWidth="27240" windowHeight="16440" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
+    <workbookView xWindow="-1680" yWindow="-27960" windowWidth="40600" windowHeight="22200" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
   </bookViews>
   <sheets>
     <sheet name="Permissions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="120">
   <si>
     <t>Group</t>
   </si>
@@ -381,13 +381,28 @@
   </si>
   <si>
     <t>submission_request:submitted</t>
+  </si>
+  <si>
+    <t>Fedlead-self</t>
+  </si>
+  <si>
+    <t>Dcp-self</t>
+  </si>
+  <si>
+    <t>Admin-self</t>
+  </si>
+  <si>
+    <t>Submitter-self</t>
+  </si>
+  <si>
+    <t>User-self</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,13 +410,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -416,8 +444,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77EC54C-AF12-1945-AE96-F02A9C2EB52A}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,40 +792,55 @@
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -822,10 +866,25 @@
         <v>12</v>
       </c>
       <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -851,10 +910,25 @@
         <v>12</v>
       </c>
       <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -880,10 +954,25 @@
         <v>12</v>
       </c>
       <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -909,10 +998,25 @@
         <v>19</v>
       </c>
       <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -938,10 +1042,25 @@
         <v>12</v>
       </c>
       <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -967,10 +1086,25 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -996,10 +1130,25 @@
         <v>19</v>
       </c>
       <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1025,10 +1174,25 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1054,10 +1218,25 @@
         <v>19</v>
       </c>
       <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1083,10 +1262,25 @@
         <v>19</v>
       </c>
       <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1112,10 +1306,25 @@
         <v>19</v>
       </c>
       <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1141,10 +1350,25 @@
         <v>19</v>
       </c>
       <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1170,10 +1394,25 @@
         <v>19</v>
       </c>
       <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1199,10 +1438,25 @@
         <v>19</v>
       </c>
       <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1228,10 +1482,25 @@
         <v>19</v>
       </c>
       <c r="I16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1257,10 +1526,25 @@
         <v>19</v>
       </c>
       <c r="I17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1286,10 +1570,25 @@
         <v>12</v>
       </c>
       <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -1315,10 +1614,25 @@
         <v>12</v>
       </c>
       <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -1344,10 +1658,25 @@
         <v>19</v>
       </c>
       <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" t="s">
+        <v>19</v>
+      </c>
+      <c r="N20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -1373,10 +1702,25 @@
         <v>12</v>
       </c>
       <c r="I21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -1402,10 +1746,25 @@
         <v>12</v>
       </c>
       <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" t="s">
+        <v>12</v>
+      </c>
+      <c r="M22" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>111</v>
       </c>
@@ -1431,10 +1790,25 @@
         <v>12</v>
       </c>
       <c r="I23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -1460,10 +1834,25 @@
         <v>12</v>
       </c>
       <c r="I24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1489,10 +1878,25 @@
         <v>19</v>
       </c>
       <c r="I25" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" t="s">
+        <v>19</v>
+      </c>
+      <c r="N25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1518,10 +1922,25 @@
         <v>19</v>
       </c>
       <c r="I26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1547,10 +1966,25 @@
         <v>19</v>
       </c>
       <c r="I27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" t="s">
+        <v>12</v>
+      </c>
+      <c r="M27" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -1576,10 +2010,25 @@
         <v>19</v>
       </c>
       <c r="I28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M28" t="s">
+        <v>19</v>
+      </c>
+      <c r="N28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -1605,10 +2054,25 @@
         <v>19</v>
       </c>
       <c r="I29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" t="s">
+        <v>12</v>
+      </c>
+      <c r="M29" t="s">
+        <v>19</v>
+      </c>
+      <c r="N29" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -1634,10 +2098,25 @@
         <v>19</v>
       </c>
       <c r="I30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" t="s">
+        <v>12</v>
+      </c>
+      <c r="M30" t="s">
+        <v>19</v>
+      </c>
+      <c r="N30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -1663,10 +2142,25 @@
         <v>19</v>
       </c>
       <c r="I31" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" t="s">
+        <v>12</v>
+      </c>
+      <c r="M31" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -1692,10 +2186,25 @@
         <v>19</v>
       </c>
       <c r="I32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" t="s">
+        <v>12</v>
+      </c>
+      <c r="M32" t="s">
+        <v>19</v>
+      </c>
+      <c r="N32" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -1721,10 +2230,25 @@
         <v>19</v>
       </c>
       <c r="I33" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M33" t="s">
+        <v>19</v>
+      </c>
+      <c r="N33" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1750,10 +2274,25 @@
         <v>19</v>
       </c>
       <c r="I34" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" t="s">
+        <v>19</v>
+      </c>
+      <c r="N34" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1779,10 +2318,25 @@
         <v>12</v>
       </c>
       <c r="I35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -1808,10 +2362,25 @@
         <v>12</v>
       </c>
       <c r="I36" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" t="s">
+        <v>12</v>
+      </c>
+      <c r="M36" t="s">
+        <v>12</v>
+      </c>
+      <c r="N36" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1837,6 +2406,21 @@
         <v>19</v>
       </c>
       <c r="I37" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" t="s">
+        <v>12</v>
+      </c>
+      <c r="L37" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" t="s">
+        <v>19</v>
+      </c>
+      <c r="N37" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PBAC WIP Phase 2
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/PBACPermissions.xlsx
+++ b/InputFiles/CRDC/PBACPermissions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/CRDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2854D568-76A7-6045-ABF4-E58D84C305F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBD46C2-A36A-7D49-BA6B-40A5295BCA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1680" yWindow="-27960" windowWidth="40600" windowHeight="22200" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="121">
   <si>
     <t>Group</t>
   </si>
@@ -396,6 +396,9 @@
   </si>
   <si>
     <t>User-self</t>
+  </si>
+  <si>
+    <t>Fedlead-positive</t>
   </si>
 </sst>
 </file>
@@ -781,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77EC54C-AF12-1945-AE96-F02A9C2EB52A}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -793,10 +796,11 @@
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,10 +841,13 @@
         <v>119</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -881,10 +888,13 @@
         <v>12</v>
       </c>
       <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -925,10 +935,13 @@
         <v>12</v>
       </c>
       <c r="N3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -969,10 +982,13 @@
         <v>12</v>
       </c>
       <c r="N4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1013,10 +1029,13 @@
         <v>19</v>
       </c>
       <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1057,10 +1076,13 @@
         <v>12</v>
       </c>
       <c r="N6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1101,10 +1123,13 @@
         <v>19</v>
       </c>
       <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1145,10 +1170,13 @@
         <v>19</v>
       </c>
       <c r="N8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1189,10 +1217,13 @@
         <v>19</v>
       </c>
       <c r="N9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1233,10 +1264,13 @@
         <v>19</v>
       </c>
       <c r="N10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1277,10 +1311,13 @@
         <v>19</v>
       </c>
       <c r="N11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1321,10 +1358,13 @@
         <v>19</v>
       </c>
       <c r="N12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1365,10 +1405,13 @@
         <v>19</v>
       </c>
       <c r="N13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1409,10 +1452,13 @@
         <v>19</v>
       </c>
       <c r="N14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1453,10 +1499,13 @@
         <v>19</v>
       </c>
       <c r="N15" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1497,10 +1546,13 @@
         <v>19</v>
       </c>
       <c r="N16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1541,10 +1593,13 @@
         <v>19</v>
       </c>
       <c r="N17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1585,10 +1640,13 @@
         <v>12</v>
       </c>
       <c r="N18" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -1629,10 +1687,13 @@
         <v>12</v>
       </c>
       <c r="N19" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -1673,10 +1734,13 @@
         <v>19</v>
       </c>
       <c r="N20" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -1717,10 +1781,13 @@
         <v>12</v>
       </c>
       <c r="N21" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -1761,10 +1828,13 @@
         <v>12</v>
       </c>
       <c r="N22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>111</v>
       </c>
@@ -1805,10 +1875,13 @@
         <v>12</v>
       </c>
       <c r="N23" t="s">
+        <v>10</v>
+      </c>
+      <c r="O23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -1849,10 +1922,13 @@
         <v>12</v>
       </c>
       <c r="N24" t="s">
+        <v>10</v>
+      </c>
+      <c r="O24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1893,10 +1969,13 @@
         <v>19</v>
       </c>
       <c r="N25" t="s">
+        <v>10</v>
+      </c>
+      <c r="O25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1937,10 +2016,13 @@
         <v>19</v>
       </c>
       <c r="N26" t="s">
+        <v>10</v>
+      </c>
+      <c r="O26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1981,10 +2063,13 @@
         <v>19</v>
       </c>
       <c r="N27" t="s">
+        <v>10</v>
+      </c>
+      <c r="O27" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -2025,10 +2110,13 @@
         <v>19</v>
       </c>
       <c r="N28" t="s">
+        <v>10</v>
+      </c>
+      <c r="O28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -2069,10 +2157,13 @@
         <v>19</v>
       </c>
       <c r="N29" t="s">
+        <v>10</v>
+      </c>
+      <c r="O29" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2113,10 +2204,13 @@
         <v>19</v>
       </c>
       <c r="N30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -2157,10 +2251,13 @@
         <v>19</v>
       </c>
       <c r="N31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -2201,10 +2298,13 @@
         <v>19</v>
       </c>
       <c r="N32" t="s">
+        <v>10</v>
+      </c>
+      <c r="O32" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2245,10 +2345,13 @@
         <v>19</v>
       </c>
       <c r="N33" t="s">
+        <v>10</v>
+      </c>
+      <c r="O33" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -2289,10 +2392,13 @@
         <v>19</v>
       </c>
       <c r="N34" t="s">
+        <v>19</v>
+      </c>
+      <c r="O34" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2333,10 +2439,13 @@
         <v>12</v>
       </c>
       <c r="N35" t="s">
+        <v>10</v>
+      </c>
+      <c r="O35" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2377,10 +2486,13 @@
         <v>12</v>
       </c>
       <c r="N36" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -2421,6 +2533,9 @@
         <v>19</v>
       </c>
       <c r="N37" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PBAC permission updates and menu relocation changes
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/PBACPermissions.xlsx
+++ b/InputFiles/CRDC/PBACPermissions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CRDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF1A525-B356-144C-ACFC-17367F30D4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A076468B-87A1-F741-912A-69DBA8324D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3280" yWindow="-27580" windowWidth="40600" windowHeight="22200" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
+    <workbookView xWindow="17080" yWindow="-24040" windowWidth="40600" windowHeight="22200" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
   </bookViews>
   <sheets>
     <sheet name="Permissions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="136">
   <si>
     <t>Group</t>
   </si>
@@ -426,6 +426,24 @@
   </si>
   <si>
     <t>Admin-negative</t>
+  </si>
+  <si>
+    <t>When pending cleared</t>
+  </si>
+  <si>
+    <t>Submission Request pending condition cleared</t>
+  </si>
+  <si>
+    <t>submission_request:pending_cleared</t>
+  </si>
+  <si>
+    <t>When New PV requested</t>
+  </si>
+  <si>
+    <t>A new PV is requested</t>
+  </si>
+  <si>
+    <t>data_submission:pv_requested</t>
   </si>
 </sst>
 </file>
@@ -855,17 +873,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77EC54C-AF12-1945-AE96-F02A9C2EB52A}">
-  <dimension ref="A1:X37"/>
+  <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -963,7 +981,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
@@ -1339,7 +1357,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -2437,10 +2455,10 @@
         <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>11</v>
@@ -2503,7 +2521,7 @@
         <v>12</v>
       </c>
       <c r="X22" s="6" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
@@ -2511,10 +2529,10 @@
         <v>111</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>11</v>
@@ -2577,7 +2595,7 @@
         <v>12</v>
       </c>
       <c r="X23" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2585,10 +2603,10 @@
         <v>111</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>11</v>
@@ -2651,48 +2669,48 @@
         <v>12</v>
       </c>
       <c r="X24" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="N25" s="5" t="s">
         <v>10</v>
@@ -2704,10 +2722,10 @@
         <v>10</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="S25" s="6" t="s">
         <v>11</v>
@@ -2719,13 +2737,13 @@
         <v>11</v>
       </c>
       <c r="V25" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="W25" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="X25" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -2733,10 +2751,10 @@
         <v>79</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>11</v>
@@ -2745,10 +2763,10 @@
         <v>10</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>19</v>
@@ -2760,10 +2778,10 @@
         <v>12</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>19</v>
@@ -2778,7 +2796,7 @@
         <v>10</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="R26" s="5" t="s">
         <v>19</v>
@@ -2793,13 +2811,13 @@
         <v>11</v>
       </c>
       <c r="V26" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="W26" s="6" t="s">
         <v>19</v>
       </c>
       <c r="X26" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
@@ -2807,10 +2825,10 @@
         <v>79</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>11</v>
@@ -2819,7 +2837,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>12</v>
@@ -2834,7 +2852,7 @@
         <v>12</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>12</v>
@@ -2873,7 +2891,7 @@
         <v>19</v>
       </c>
       <c r="X27" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
@@ -2881,10 +2899,10 @@
         <v>79</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>11</v>
@@ -2893,7 +2911,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>12</v>
@@ -2908,7 +2926,7 @@
         <v>12</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>12</v>
@@ -2947,7 +2965,7 @@
         <v>19</v>
       </c>
       <c r="X28" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
@@ -2955,10 +2973,10 @@
         <v>79</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>11</v>
@@ -2967,7 +2985,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>12</v>
@@ -2982,7 +3000,7 @@
         <v>12</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>12</v>
@@ -3021,7 +3039,7 @@
         <v>19</v>
       </c>
       <c r="X29" s="6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
@@ -3029,10 +3047,10 @@
         <v>79</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>11</v>
@@ -3095,7 +3113,7 @@
         <v>19</v>
       </c>
       <c r="X30" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
@@ -3103,10 +3121,10 @@
         <v>79</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>11</v>
@@ -3169,7 +3187,7 @@
         <v>19</v>
       </c>
       <c r="X31" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
@@ -3177,10 +3195,10 @@
         <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>11</v>
@@ -3243,7 +3261,7 @@
         <v>19</v>
       </c>
       <c r="X32" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
@@ -3251,10 +3269,10 @@
         <v>79</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>11</v>
@@ -3317,30 +3335,30 @@
         <v>19</v>
       </c>
       <c r="X33" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>19</v>
@@ -3349,90 +3367,90 @@
         <v>19</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>19</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="P34" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q34" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="R34" s="5" t="s">
         <v>19</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="T34" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="U34" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V34" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="W34" s="6" t="s">
         <v>19</v>
       </c>
       <c r="X34" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N35" s="5" t="s">
         <v>10</v>
@@ -3444,10 +3462,10 @@
         <v>10</v>
       </c>
       <c r="Q35" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="R35" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="S35" s="6" t="s">
         <v>11</v>
@@ -3459,13 +3477,13 @@
         <v>11</v>
       </c>
       <c r="V35" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="W35" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="X35" s="6" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
@@ -3473,73 +3491,73 @@
         <v>56</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q36" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="R36" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="U36" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="W36" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="X36" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
@@ -3547,72 +3565,220 @@
         <v>56</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="U37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="W37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="X37" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="W38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="X38" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="R37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="S37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="T37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="W37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="X37" s="6" t="s">
+      <c r="D39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="W39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X39" s="6" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new PBAC permission - When config changed- and add label verifications
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/PBACPermissions.xlsx
+++ b/InputFiles/CRDC/PBACPermissions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CRDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A076468B-87A1-F741-912A-69DBA8324D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173F9B59-AFB3-354B-8AEE-645076B667C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="-24040" windowWidth="40600" windowHeight="22200" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
+    <workbookView xWindow="3300" yWindow="-25440" windowWidth="40600" windowHeight="22200" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
   </bookViews>
   <sheets>
     <sheet name="Permissions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="139">
   <si>
     <t>Group</t>
   </si>
@@ -444,6 +444,15 @@
   </si>
   <si>
     <t>data_submission:pv_requested</t>
+  </si>
+  <si>
+    <t>Configuration is changed</t>
+  </si>
+  <si>
+    <t>data_submission:cfg_changed</t>
+  </si>
+  <si>
+    <t>When config changed</t>
   </si>
 </sst>
 </file>
@@ -873,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77EC54C-AF12-1945-AE96-F02A9C2EB52A}">
-  <dimension ref="A1:X39"/>
+  <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3488,25 +3497,25 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>19</v>
@@ -3515,49 +3524,49 @@
         <v>19</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>19</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q36" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="R36" s="5" t="s">
         <v>19</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="U36" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="W36" s="6" t="s">
         <v>19</v>
       </c>
       <c r="X36" s="6" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
@@ -3565,73 +3574,73 @@
         <v>56</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q37" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="S37" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="U37" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="V37" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="W37" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="X37" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
@@ -3639,16 +3648,16 @@
         <v>56</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>10</v>
@@ -3675,10 +3684,10 @@
         <v>12</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>10</v>
@@ -3690,10 +3699,10 @@
         <v>12</v>
       </c>
       <c r="S38" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U38" s="6" t="s">
         <v>11</v>
@@ -3705,7 +3714,7 @@
         <v>12</v>
       </c>
       <c r="X38" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
@@ -3713,72 +3722,146 @@
         <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="W39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="X39" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P39" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q39" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="R39" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="S39" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="T39" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V39" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="W39" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="X39" s="6" t="s">
+      <c r="D40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="W40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X40" s="6" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix expected PBAC permission for Submitter and change IU federation source id
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/PBACPermissions.xlsx
+++ b/InputFiles/CRDC/PBACPermissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CRDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173F9B59-AFB3-354B-8AEE-645076B667C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C462BE7-B02B-5C48-B2D4-CE0E1584D05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="-25440" windowWidth="40600" windowHeight="22200" xr2:uid="{94E754EE-2D10-D84B-9E75-EAF6D371D76A}"/>
   </bookViews>
@@ -3515,7 +3515,7 @@
         <v>11</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>19</v>
@@ -3545,7 +3545,7 @@
         <v>10</v>
       </c>
       <c r="Q36" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R36" s="5" t="s">
         <v>19</v>
@@ -3560,7 +3560,7 @@
         <v>11</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="W36" s="6" t="s">
         <v>19</v>

</xml_diff>